<commit_message>
Added analytics tools for admin panel
</commit_message>
<xml_diff>
--- a/data/database_backup/users.xlsx
+++ b/data/database_backup/users.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +464,21 @@
           <t>uik</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>role</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>register_date</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>consultant_rating</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -494,9 +509,66 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>gfff422</t>
-        </is>
-      </c>
+          <t>Елса100</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>consultant</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2023-07-01</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>1701092781</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>zhm1603</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Чел</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>КААЙ206</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>user</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>2023-07-01</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>